<commit_message>
inicio de esquematico do projeto com eplan
</commit_message>
<xml_diff>
--- a/descritivo/Lista_IO.xlsx
+++ b/descritivo/Lista_IO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\livros projeto\exemplos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\proj_MPM\MPM300\descritivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,9 +77,6 @@
     <t>solenóides</t>
   </si>
   <si>
-    <t>32x válvulas das massas</t>
-  </si>
-  <si>
     <t>Válvula do varão</t>
   </si>
   <si>
@@ -125,12 +122,6 @@
     <t>Acionamento de emergência</t>
   </si>
   <si>
-    <t>Saídas - 39</t>
-  </si>
-  <si>
-    <t>4x transdutor de pressão</t>
-  </si>
-  <si>
     <t>posição de arquisição do varão</t>
   </si>
   <si>
@@ -141,6 +132,15 @@
   </si>
   <si>
     <t>posição máxima do varão</t>
+  </si>
+  <si>
+    <t>16x válvulas das massas</t>
+  </si>
+  <si>
+    <t>Saídas - 23</t>
+  </si>
+  <si>
+    <t>3x transdutor de pressão</t>
   </si>
 </sst>
 </file>
@@ -257,10 +257,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
@@ -547,7 +547,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,15 +561,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D1" s="10"/>
-      <c r="E1" s="11" t="s">
-        <v>23</v>
+      <c r="E1" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -585,12 +585,12 @@
       <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="12"/>
       <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -606,11 +606,11 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="12"/>
       <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="12"/>
+        <v>24</v>
+      </c>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -625,11 +625,11 @@
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -639,69 +639,69 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="12"/>
       <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="12"/>
       <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="E7" s="12"/>
       <c r="G7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -711,12 +711,12 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -726,12 +726,12 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -742,7 +742,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -753,18 +753,18 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="11"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -775,7 +775,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
etapa anterior ao desenho dos esquematicos das fontes de alimentacao,
</commit_message>
<xml_diff>
--- a/descritivo/Lista_IO.xlsx
+++ b/descritivo/Lista_IO.xlsx
@@ -56,9 +56,6 @@
     <t>analógica</t>
   </si>
   <si>
-    <t>analógico, extensômetro</t>
-  </si>
-  <si>
     <t>módulo wifi</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>3x transdutor de pressão</t>
+  </si>
+  <si>
+    <t>extensômetro e potenciômetro</t>
   </si>
 </sst>
 </file>
@@ -547,12 +547,12 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -561,15 +561,15 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,10 +587,10 @@
       </c>
       <c r="E2" s="12"/>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
       </c>
       <c r="E3" s="12"/>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="11"/>
     </row>
@@ -627,79 +627,79 @@
       </c>
       <c r="E4" s="12"/>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="12"/>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="12"/>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="12"/>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="12"/>
     </row>
@@ -711,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -720,22 +720,22 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>9</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>9</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>9</v>
@@ -768,10 +768,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2"/>

</xml_diff>

<commit_message>
inicio de insercao de componentes 2d de fabricantes, e dimensionamento dos paineis e caixas de juncao
</commit_message>
<xml_diff>
--- a/descritivo/Lista_IO.xlsx
+++ b/descritivo/Lista_IO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Descrição</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>extensômetro e potenciômetro</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -233,7 +236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -262,6 +265,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,6 +783,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="12"/>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>

</xml_diff>